<commit_message>
Cập nhật file product, thêm folder chứa mẫu ảnh cho DTCC
</commit_message>
<xml_diff>
--- a/preparation/Product.xlsx
+++ b/preparation/Product.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Learning\Lập trình trực quan\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49428C7-4ACA-45DE-9C52-42EBFB7CE626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BB6B18-B24E-487A-BA69-3E1AB19D7BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="1" r:id="rId1"/>
-    <sheet name="Provider" sheetId="2" r:id="rId2"/>
-    <sheet name="Clients" sheetId="3" r:id="rId3"/>
+    <sheet name="SANPHAM" sheetId="1" r:id="rId1"/>
+    <sheet name="NHANVIEN" sheetId="4" r:id="rId2"/>
+    <sheet name="DTCC" sheetId="2" r:id="rId3"/>
+    <sheet name="KHACHHANG" sheetId="3" r:id="rId4"/>
+    <sheet name="CALAM" sheetId="6" r:id="rId5"/>
+    <sheet name="CT_LAMVIEC" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="383">
   <si>
     <t>STT</t>
   </si>
@@ -949,6 +952,261 @@
   </si>
   <si>
     <t>Link minh họa: https://drive.google.com/file/d/17w09gSmW_3U1O9XgQz822lMGhE26eFaU/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Ngày vào làm</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Ngày sinh</t>
+  </si>
+  <si>
+    <t>Thưởng</t>
+  </si>
+  <si>
+    <t>NV01</t>
+  </si>
+  <si>
+    <t>NV02</t>
+  </si>
+  <si>
+    <t>NV03</t>
+  </si>
+  <si>
+    <t>NV04</t>
+  </si>
+  <si>
+    <t>NV05</t>
+  </si>
+  <si>
+    <t>NV06</t>
+  </si>
+  <si>
+    <t>Lê Thị Bống</t>
+  </si>
+  <si>
+    <t>0255 968 968</t>
+  </si>
+  <si>
+    <t>Thu ngân</t>
+  </si>
+  <si>
+    <t>6.000.000đ</t>
+  </si>
+  <si>
+    <t>Trần Dần</t>
+  </si>
+  <si>
+    <t>0983 455 266</t>
+  </si>
+  <si>
+    <t>30/7/2015</t>
+  </si>
+  <si>
+    <t>16/6/1975</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Kỹ thuật viên</t>
+  </si>
+  <si>
+    <t>Tư vấn viên</t>
+  </si>
+  <si>
+    <t>0777 865 432</t>
+  </si>
+  <si>
+    <t>31/12/2016</t>
+  </si>
+  <si>
+    <t>17/7/2002</t>
+  </si>
+  <si>
+    <t>Quách Siêu Sang</t>
+  </si>
+  <si>
+    <t>0346 156 112</t>
+  </si>
+  <si>
+    <t>31/5/2016</t>
+  </si>
+  <si>
+    <t>30/4/2002</t>
+  </si>
+  <si>
+    <t>Đoàn Thị Kim Liên</t>
+  </si>
+  <si>
+    <t>Lê Minh Quang</t>
+  </si>
+  <si>
+    <t>0923 456 442</t>
+  </si>
+  <si>
+    <t>Lê Thị Nở</t>
+  </si>
+  <si>
+    <t>0999 943 349</t>
+  </si>
+  <si>
+    <t>22/7/2016</t>
+  </si>
+  <si>
+    <t>Mã ca</t>
+  </si>
+  <si>
+    <t>Thứ</t>
+  </si>
+  <si>
+    <t>Giờ bắt đầu</t>
+  </si>
+  <si>
+    <t>Giờ nghỉ</t>
+  </si>
+  <si>
+    <t>C2S</t>
+  </si>
+  <si>
+    <t>C2C</t>
+  </si>
+  <si>
+    <t>C2T</t>
+  </si>
+  <si>
+    <t>C3S</t>
+  </si>
+  <si>
+    <t>C3C</t>
+  </si>
+  <si>
+    <t>C3T</t>
+  </si>
+  <si>
+    <t>C4S</t>
+  </si>
+  <si>
+    <t>C4C</t>
+  </si>
+  <si>
+    <t>C4T</t>
+  </si>
+  <si>
+    <t>C5S</t>
+  </si>
+  <si>
+    <t>C5C</t>
+  </si>
+  <si>
+    <t>C5T</t>
+  </si>
+  <si>
+    <t>C6S</t>
+  </si>
+  <si>
+    <t>C6C</t>
+  </si>
+  <si>
+    <t>C6T</t>
+  </si>
+  <si>
+    <t>C7S</t>
+  </si>
+  <si>
+    <t>C7C</t>
+  </si>
+  <si>
+    <t>C7T</t>
+  </si>
+  <si>
+    <t>C8S</t>
+  </si>
+  <si>
+    <t>C8C</t>
+  </si>
+  <si>
+    <t>C8T</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>7h30</t>
+  </si>
+  <si>
+    <t>11h</t>
+  </si>
+  <si>
+    <t>13h30</t>
+  </si>
+  <si>
+    <t>17h</t>
+  </si>
+  <si>
+    <t>17h30</t>
+  </si>
+  <si>
+    <t>21h</t>
+  </si>
+  <si>
+    <t>Mã ca = C + "Thứ" (từ 2-8) + ca.</t>
+  </si>
+  <si>
+    <t>Ca 1: Sáng (S) | 7h30 - 11h</t>
+  </si>
+  <si>
+    <t>Ca 2: Chiều (C) | 13h30 - 17h</t>
+  </si>
+  <si>
+    <t>Ca 3: Tối (T) | 17h30 - 21h</t>
+  </si>
+  <si>
+    <t>Mã nhân viên</t>
+  </si>
+  <si>
+    <t>Ngày làm</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Chức vụ</t>
+  </si>
+  <si>
+    <t>Chủ tiệm</t>
+  </si>
+  <si>
+    <t>Tên đăng nhập</t>
+  </si>
+  <si>
+    <t>0255968968</t>
+  </si>
+  <si>
+    <t>0983455266</t>
+  </si>
+  <si>
+    <t>0777865432</t>
+  </si>
+  <si>
+    <t>0346156112</t>
+  </si>
+  <si>
+    <t>0923456442</t>
+  </si>
+  <si>
+    <t>0999943349</t>
+  </si>
+  <si>
+    <t>Lương</t>
+  </si>
+  <si>
+    <t>8.000.000đ</t>
+  </si>
+  <si>
+    <t>Mật khẩu</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1071,6 +1329,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1354,7 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -2989,6 +3256,342 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512C9807-2171-46C3-A68C-A0E26548160E}">
+  <dimension ref="A4:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="27.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" s="9">
+        <v>42370</v>
+      </c>
+      <c r="F5" s="9">
+        <v>29560</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>374</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="K5" s="15">
+        <v>123456</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>375</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="K6" s="15">
+        <v>123456</v>
+      </c>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="J7" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="K7" s="15">
+        <v>123456</v>
+      </c>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="J8" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="K8" s="15">
+        <v>123456</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E9" s="9">
+        <v>42709</v>
+      </c>
+      <c r="F9" s="9">
+        <v>36809</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>381</v>
+      </c>
+      <c r="J9" s="15">
+        <v>0.12</v>
+      </c>
+      <c r="K9" s="15">
+        <v>123456</v>
+      </c>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="F10" s="14">
+        <v>37137</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="H10" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0</v>
+      </c>
+      <c r="K10" s="15">
+        <v>123456</v>
+      </c>
+      <c r="L10" s="10"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5B0F30-7841-491D-8249-626A041BB655}">
   <dimension ref="A4:F26"/>
   <sheetViews>
@@ -3216,7 +3819,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C25056B-C7B7-4F76-B500-DDAA14007CC3}">
   <dimension ref="A3:I19"/>
   <sheetViews>
@@ -3478,4 +4081,563 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631D18A0-5369-4161-942C-047038DEADCC}">
+  <dimension ref="C6:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="1">
+        <v>5</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E12" s="1">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E16" s="1">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1">
+        <v>12</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E19" s="1">
+        <v>6</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>14</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E20" s="1">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="E21" s="1">
+        <v>6</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="1">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="E22" s="1">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="1">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="E23" s="1">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="1">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="E24" s="1">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="1">
+        <v>19</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="1">
+        <v>20</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="1">
+        <v>21</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C74F319-80BF-4E3F-A0A7-639B00BCC681}">
+  <dimension ref="C5:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J22" sqref="J22:J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cập nhật file product. Thêm các samples cho DTCC
</commit_message>
<xml_diff>
--- a/preparation/Product.xlsx
+++ b/preparation/Product.xlsx
@@ -5,20 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Learning\Lập trình trực quan\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\GUI Project\DO-AN-NHOM-1\preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BB6B18-B24E-487A-BA69-3E1AB19D7BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4AB1AD-CB4F-464D-A1D4-F808BD469FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SANPHAM" sheetId="1" r:id="rId1"/>
     <sheet name="NHANVIEN" sheetId="4" r:id="rId2"/>
     <sheet name="DTCC" sheetId="2" r:id="rId3"/>
     <sheet name="KHACHHANG" sheetId="3" r:id="rId4"/>
-    <sheet name="CALAM" sheetId="6" r:id="rId5"/>
-    <sheet name="CT_LAMVIEC" sheetId="7" r:id="rId6"/>
+    <sheet name="LOAIKH" sheetId="8" r:id="rId5"/>
+    <sheet name="CALAM" sheetId="6" r:id="rId6"/>
+    <sheet name="CT_LAMVIEC" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="399">
   <si>
     <t>STT</t>
   </si>
@@ -1207,6 +1208,54 @@
   </si>
   <si>
     <t>Mật khẩu</t>
+  </si>
+  <si>
+    <t>346 Quãng Trường Dân Chủ, quận Bình Thạnh, thành phố HCM</t>
+  </si>
+  <si>
+    <t>NOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tên loại </t>
+  </si>
+  <si>
+    <t>Ưu đãi</t>
+  </si>
+  <si>
+    <t>Đặc biệt</t>
+  </si>
+  <si>
+    <t>Tặng balo khi mua laptop. Bảo hành 6 tháng cho các linh kiện điện tử, máy tính. Bảo hành 1 năm cho dòng sản phẩm laptop, 2 năm nếu khách hàng là sinh viên. Giảm giá ưu đãi nhân các dịp đặc biệt.</t>
+  </si>
+  <si>
+    <t>Tặng balo khi mua laptop. Bảo hành 6 tháng cho các linh kiện điện tử, máy tính. Bảo hành 1 năm cho dòng sản phẩm laptop, 2 năm nếu khách hàng là sinh viên. Giảm giá ưu đãi nhân các dịp đặc biệt. Được tặng kèo voucher giảm giá cho những lần mua hàng sau.</t>
+  </si>
+  <si>
+    <t>QL13, Lái Thiêu, Thuận An, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>465A QL13, Khu phố Nguyễn Trãi, P, Bình Dương 75000, Việt Nam</t>
+  </si>
+  <si>
+    <t>WMRQ+7J9, Hưng Định, Thuận An, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>XM76+C2C, Chánh Nghĩa, Thủ Dầu Một, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>132 Đ. Nguyễn Văn Lộng, Chánh Mỹ, Thủ Dầu Một, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>171 ĐX 082, Định Hoà, Thủ Dầu Một, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>Số 270 Đường ĐX064, Định Hoà, Thủ Dầu Một, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>Quốc Lộ 13, Phường Tân Định, Bến Cát, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>20 Dân Chủ, Hoà Lợi, Bến Cát, Bình Dương, Việt Nam</t>
   </si>
 </sst>
 </file>
@@ -1240,7 +1289,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1285,11 +1334,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1337,6 +1397,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3259,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{512C9807-2171-46C3-A68C-A0E26548160E}">
   <dimension ref="A4:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3593,10 +3659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5B0F30-7841-491D-8249-626A041BB655}">
-  <dimension ref="A4:F26"/>
+  <dimension ref="A4:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I16:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3604,10 +3670,11 @@
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" customWidth="1"/>
+    <col min="7" max="7" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -3623,11 +3690,14 @@
       <c r="E4" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -3643,9 +3713,12 @@
       <c r="E5" s="9">
         <v>42923</v>
       </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -3661,9 +3734,12 @@
       <c r="E6" s="9">
         <v>42710</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="9" t="s">
+        <v>390</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>3</v>
       </c>
@@ -3679,9 +3755,12 @@
       <c r="E7" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -3697,9 +3776,12 @@
       <c r="E8" s="9">
         <v>42736</v>
       </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -3715,9 +3797,12 @@
       <c r="E9" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>6</v>
       </c>
@@ -3733,9 +3818,12 @@
       <c r="E10" s="9">
         <v>42624</v>
       </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="9" t="s">
+        <v>394</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7</v>
       </c>
@@ -3751,9 +3839,12 @@
       <c r="E11" s="9">
         <v>42654</v>
       </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8</v>
       </c>
@@ -3769,9 +3860,12 @@
       <c r="E12" s="9">
         <v>42830</v>
       </c>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -3787,9 +3881,12 @@
       <c r="E13" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -3805,7 +3902,10 @@
       <c r="E14" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="G14" s="7"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
@@ -3824,7 +3924,7 @@
   <dimension ref="A3:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3890,7 +3990,7 @@
         <v>264</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -3944,7 +4044,7 @@
         <v>277</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -3998,7 +4098,7 @@
         <v>292</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -4025,7 +4125,7 @@
         <v>296</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>265</v>
+        <v>384</v>
       </c>
       <c r="I9" s="10"/>
     </row>
@@ -4084,6 +4184,73 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0A7FA1-9C57-46B4-BA5E-F5C1283532C5}">
+  <dimension ref="D6:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="8" width="33.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>388</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="4:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="H8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{631D18A0-5369-4161-942C-047038DEADCC}">
   <dimension ref="C6:G35"/>
   <sheetViews>
@@ -4513,7 +4680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C74F319-80BF-4E3F-A0A7-639B00BCC681}">
   <dimension ref="C5:G18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Cập nhật tab khách hàng. Cập nhật file product (thay đổi mã khách hàng)
</commit_message>
<xml_diff>
--- a/preparation/Product.xlsx
+++ b/preparation/Product.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\GUI Project\DO-AN-NHOM-1\preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4AB1AD-CB4F-464D-A1D4-F808BD469FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BC6C7F-FA29-4470-8887-65712BCD4787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SANPHAM" sheetId="1" r:id="rId1"/>
@@ -859,21 +859,12 @@
     <t>Thường</t>
   </si>
   <si>
-    <t>RCNOR035</t>
-  </si>
-  <si>
-    <t>RCVIP013</t>
-  </si>
-  <si>
     <t>Nguyễn Trung Kiên</t>
   </si>
   <si>
     <t>Khu phố 6, KTX khu A ĐHQG HCM</t>
   </si>
   <si>
-    <t>0777 747 1457</t>
-  </si>
-  <si>
     <t>29/2/2016</t>
   </si>
   <si>
@@ -898,9 +889,6 @@
     <t>20/2/2016</t>
   </si>
   <si>
-    <t>RCNOR019</t>
-  </si>
-  <si>
     <t>Danny Nguyễn</t>
   </si>
   <si>
@@ -913,9 +901,6 @@
     <t>30.478.000đ</t>
   </si>
   <si>
-    <t>RCVIP745</t>
-  </si>
-  <si>
     <t>*Các địa chỉ và số điện thoại trên chỉ là tự suy ra, có khả năng sai và không tồn tại.</t>
   </si>
   <si>
@@ -928,9 +913,6 @@
     <t>Ngày ký (DD/MM/YYYY)</t>
   </si>
   <si>
-    <t>RCNOR103</t>
-  </si>
-  <si>
     <t>Nguyễn Phùng Vân</t>
   </si>
   <si>
@@ -940,9 +922,6 @@
     <t>1.950.400</t>
   </si>
   <si>
-    <t>RCNOR122</t>
-  </si>
-  <si>
     <t>Trịnh Thị Nở</t>
   </si>
   <si>
@@ -1256,6 +1235,27 @@
   </si>
   <si>
     <t>20 Dân Chủ, Hoà Lợi, Bến Cát, Bình Dương, Việt Nam</t>
+  </si>
+  <si>
+    <t>RC01</t>
+  </si>
+  <si>
+    <t>RC02</t>
+  </si>
+  <si>
+    <t>RC03</t>
+  </si>
+  <si>
+    <t>RC04</t>
+  </si>
+  <si>
+    <t>RC05</t>
+  </si>
+  <si>
+    <t>RC06</t>
+  </si>
+  <si>
+    <t>0777 471 457</t>
   </si>
 </sst>
 </file>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" s="13" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3352,28 +3352,28 @@
         <v>256</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>11</v>
@@ -3384,13 +3384,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>302</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>309</v>
       </c>
       <c r="E5" s="9">
         <v>42370</v>
@@ -3399,13 +3399,13 @@
         <v>29560</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="J5" s="15">
         <v>0.05</v>
@@ -3420,31 +3420,31 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="K6" s="15">
         <v>123456</v>
@@ -3456,28 +3456,28 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>369</v>
+      </c>
+      <c r="I7" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>376</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>311</v>
       </c>
       <c r="J7" s="15">
         <v>0.1</v>
@@ -3492,28 +3492,28 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="J8" s="15">
         <v>0.1</v>
@@ -3528,13 +3528,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E9" s="9">
         <v>42709</v>
@@ -3543,13 +3543,13 @@
         <v>36809</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="J9" s="15">
         <v>0.12</v>
@@ -3564,28 +3564,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="F10" s="14">
         <v>37137</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="J10" s="16">
         <v>0</v>
@@ -3661,7 +3661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE5B0F30-7841-491D-8249-626A041BB655}">
   <dimension ref="A4:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I16:I17"/>
     </sheetView>
   </sheetViews>
@@ -3688,7 +3688,7 @@
         <v>221</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>257</v>
@@ -3714,7 +3714,7 @@
         <v>42923</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -3735,7 +3735,7 @@
         <v>42710</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -3756,7 +3756,7 @@
         <v>236</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="G7" s="7"/>
     </row>
@@ -3777,7 +3777,7 @@
         <v>42736</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="G8" s="7"/>
     </row>
@@ -3795,10 +3795,10 @@
         <v>239</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G9" s="7"/>
     </row>
@@ -3819,7 +3819,7 @@
         <v>42624</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -3840,7 +3840,7 @@
         <v>42654</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="G11" s="7"/>
     </row>
@@ -3861,7 +3861,7 @@
         <v>42830</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="G12" s="7"/>
     </row>
@@ -3882,7 +3882,7 @@
         <v>251</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="G13" s="7"/>
     </row>
@@ -3903,13 +3903,13 @@
         <v>254</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="G14" s="7"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3923,8 +3923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C25056B-C7B7-4F76-B500-DDAA14007CC3}">
   <dimension ref="A3:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3972,7 +3972,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>266</v>
+        <v>392</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>261</v>
@@ -3990,7 +3990,7 @@
         <v>264</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -3999,25 +3999,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>273</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -4026,25 +4026,25 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>279</v>
+        <v>394</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -4053,25 +4053,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>284</v>
+        <v>395</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -4080,25 +4080,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>289</v>
+        <v>396</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -4106,26 +4106,26 @@
       <c r="A9" s="10">
         <v>6</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>293</v>
+      <c r="B9" s="1" t="s">
+        <v>397</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="I9" s="10"/>
     </row>
@@ -4175,10 +4175,11 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4198,7 +4199,7 @@
     <col min="7" max="8" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D6" s="1" t="s">
         <v>0</v>
       </c>
@@ -4206,10 +4207,10 @@
         <v>260</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -4220,13 +4221,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>265</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -4235,13 +4236,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -4271,16 +4272,16 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
@@ -4288,16 +4289,16 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
@@ -4305,16 +4306,16 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
@@ -4322,16 +4323,16 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
@@ -4339,16 +4340,16 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
@@ -4356,16 +4357,16 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
@@ -4373,16 +4374,16 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
@@ -4390,16 +4391,16 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="E13" s="1">
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
@@ -4407,16 +4408,16 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
@@ -4424,16 +4425,16 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="E15" s="1">
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
@@ -4441,16 +4442,16 @@
         <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="E16" s="1">
         <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
@@ -4458,16 +4459,16 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
@@ -4475,16 +4476,16 @@
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="E18" s="1">
         <v>5</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
@@ -4492,16 +4493,16 @@
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="E19" s="1">
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
@@ -4509,16 +4510,16 @@
         <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="E20" s="1">
         <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
@@ -4526,16 +4527,16 @@
         <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="E21" s="1">
         <v>6</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
@@ -4543,16 +4544,16 @@
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="E22" s="1">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
@@ -4560,16 +4561,16 @@
         <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="E23" s="1">
         <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
@@ -4577,16 +4578,16 @@
         <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="E24" s="1">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
@@ -4594,16 +4595,16 @@
         <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
@@ -4611,16 +4612,16 @@
         <v>20</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
@@ -4628,16 +4629,16 @@
         <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
@@ -4656,22 +4657,22 @@
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -4701,16 +4702,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Hoàn thành phần khách hàng đăng kí và đã hoàn thành chức năng tạo ưu đãi.
</commit_message>
<xml_diff>
--- a/preparation/Product.xlsx
+++ b/preparation/Product.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\GUI Project\DO-AN-NHOM-1\preparation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BC6C7F-FA29-4470-8887-65712BCD4787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5D83D7-1B64-41EA-BD73-91D82B7047AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SANPHAM" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="400">
   <si>
     <t>STT</t>
   </si>
@@ -661,9 +661,6 @@
     <t>SSD Samsung 860 Evo 250GB 2.5" Sata 3 550/520 MB/s ( MZ-76E250BW )</t>
   </si>
   <si>
-    <t>Ổ cứng</t>
-  </si>
-  <si>
     <t>HDS963</t>
   </si>
   <si>
@@ -1256,6 +1253,12 @@
   </si>
   <si>
     <t>0777 471 457</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>HDD</t>
   </si>
 </sst>
 </file>
@@ -1687,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:M47"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3159,19 +3162,19 @@
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>199</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>200</v>
+        <v>398</v>
       </c>
       <c r="E40" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F40" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>161</v>
@@ -3189,7 +3192,7 @@
         <v>20</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M40" s="1"/>
     </row>
@@ -3198,13 +3201,13 @@
         <v>38</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>200</v>
+        <v>398</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>144</v>
@@ -3228,7 +3231,7 @@
         <v>10</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M41" s="1"/>
     </row>
@@ -3237,22 +3240,22 @@
         <v>39</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E42" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>176</v>
@@ -3267,7 +3270,7 @@
         <v>30</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="M42" s="1"/>
     </row>
@@ -3276,25 +3279,25 @@
         <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>50</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>16</v>
@@ -3306,13 +3309,13 @@
         <v>10</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="M43" s="1"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B47" s="13" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -3346,34 +3349,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>294</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>11</v>
@@ -3384,13 +3387,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>302</v>
       </c>
       <c r="E5" s="9">
         <v>42370</v>
@@ -3399,13 +3402,13 @@
         <v>29560</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>366</v>
+      </c>
+      <c r="I5" s="15" t="s">
         <v>303</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>367</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>304</v>
       </c>
       <c r="J5" s="15">
         <v>0.05</v>
@@ -3420,31 +3423,31 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="I6" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>368</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>309</v>
-      </c>
       <c r="J6" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K6" s="15">
         <v>123456</v>
@@ -3456,28 +3459,28 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>312</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>313</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>314</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J7" s="15">
         <v>0.1</v>
@@ -3492,28 +3495,28 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J8" s="15">
         <v>0.1</v>
@@ -3528,13 +3531,13 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="E9" s="9">
         <v>42709</v>
@@ -3543,13 +3546,13 @@
         <v>36809</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="J9" s="15">
         <v>0.12</v>
@@ -3564,28 +3567,28 @@
         <v>6</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>322</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="E10" s="10" t="s">
         <v>323</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>324</v>
       </c>
       <c r="F10" s="14">
         <v>37137</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J10" s="16">
         <v>0</v>
@@ -3679,19 +3682,19 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>221</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G4" s="7" t="s">
         <v>11</v>
@@ -3702,19 +3705,19 @@
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E5" s="9">
         <v>42923</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G5" s="7"/>
     </row>
@@ -3723,19 +3726,19 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E6" s="9">
         <v>42710</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -3744,19 +3747,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>236</v>
-      </c>
       <c r="F7" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G7" s="7"/>
     </row>
@@ -3765,19 +3768,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E8" s="9">
         <v>42736</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G8" s="7"/>
     </row>
@@ -3786,19 +3789,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>239</v>
-      </c>
       <c r="E9" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G9" s="7"/>
     </row>
@@ -3807,19 +3810,19 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>244</v>
       </c>
       <c r="E10" s="9">
         <v>42624</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -3828,19 +3831,19 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="E11" s="9">
         <v>42654</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G11" s="7"/>
     </row>
@@ -3849,19 +3852,19 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="E12" s="9">
         <v>42830</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G12" s="7"/>
     </row>
@@ -3870,19 +3873,19 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="9" t="s">
         <v>250</v>
       </c>
-      <c r="E13" s="9" t="s">
-        <v>251</v>
-      </c>
       <c r="F13" s="9" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G13" s="7"/>
     </row>
@@ -3891,25 +3894,25 @@
         <v>10</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>254</v>
-      </c>
       <c r="F14" s="9" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G14" s="7"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -3923,7 +3926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C25056B-C7B7-4F76-B500-DDAA14007CC3}">
   <dimension ref="A3:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -3943,25 +3946,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>260</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>11</v>
@@ -3972,25 +3975,25 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="F4" s="9">
         <v>42767</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -3999,25 +4002,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>270</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -4026,25 +4029,25 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I6" s="1"/>
     </row>
@@ -4053,25 +4056,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I7" s="1"/>
     </row>
@@ -4080,25 +4083,25 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I8" s="1"/>
     </row>
@@ -4107,25 +4110,25 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C9" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>267</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="F9" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>289</v>
-      </c>
       <c r="H9" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I9" s="10"/>
     </row>
@@ -4175,7 +4178,7 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -4204,13 +4207,13 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
@@ -4221,13 +4224,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H7" s="1"/>
     </row>
@@ -4236,13 +4239,13 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -4272,16 +4275,16 @@
         <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
@@ -4289,16 +4292,16 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
@@ -4306,16 +4309,16 @@
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
@@ -4323,16 +4326,16 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
@@ -4340,16 +4343,16 @@
         <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E10" s="1">
         <v>3</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
@@ -4357,16 +4360,16 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E11" s="1">
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
@@ -4374,16 +4377,16 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E12" s="1">
         <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
@@ -4391,16 +4394,16 @@
         <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E13" s="1">
         <v>4</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
@@ -4408,16 +4411,16 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
@@ -4425,16 +4428,16 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E15" s="1">
         <v>4</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
@@ -4442,16 +4445,16 @@
         <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E16" s="1">
         <v>5</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
@@ -4459,16 +4462,16 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
@@ -4476,16 +4479,16 @@
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E18" s="1">
         <v>5</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
@@ -4493,16 +4496,16 @@
         <v>13</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E19" s="1">
         <v>6</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
@@ -4510,16 +4513,16 @@
         <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E20" s="1">
         <v>6</v>
       </c>
       <c r="F20" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
@@ -4527,16 +4530,16 @@
         <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E21" s="1">
         <v>6</v>
       </c>
       <c r="F21" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
@@ -4544,16 +4547,16 @@
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E22" s="1">
         <v>7</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
@@ -4561,16 +4564,16 @@
         <v>17</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E23" s="1">
         <v>7</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
@@ -4578,16 +4581,16 @@
         <v>18</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E24" s="1">
         <v>7</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
@@ -4595,16 +4598,16 @@
         <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E25" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
@@ -4612,16 +4615,16 @@
         <v>20</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>353</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
@@ -4629,16 +4632,16 @@
         <v>21</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>350</v>
-      </c>
       <c r="F27" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="G27" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
@@ -4657,22 +4660,22 @@
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G35" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -4702,16 +4705,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>